<commit_message>
- Adapté l'importation pour pouvoir importer des fichiers qui ne sont pas associés à une paroisse ou à une région spécifique. En gros, on rajoute une propriété Kind à EervId qui indique s'il s'agit de données cantonales, régionales ou paroissiales. Cela remplace la propriété IsParish. Ce qui implique des modifications partous là où cette propriété était utilisée. Cela implique aussi de rajouter une colonne dans les fichiers d'ids pour indiquer de quel type est un id.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@20312 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/App.Aider/Samples/EERV Morges/Ids.xlsx
+++ b/Epsitec.Cresus/App.Aider/Samples/EERV Morges/Ids.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="15615" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>_id</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>Morges</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
@@ -442,15 +448,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,8 +475,11 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -489,8 +498,11 @@
       <c r="F2" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
@@ -498,7 +510,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
@@ -506,7 +518,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
@@ -514,7 +526,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
@@ -522,7 +534,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
@@ -530,7 +542,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
     </row>

</xml_diff>